<commit_message>
update controlled vocabulary in data files
</commit_message>
<xml_diff>
--- a/data/vgp_database/Bighorn_Basin_sediments.xlsx
+++ b/data/vgp_database/Bighorn_Basin_sediments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yimingzhang/Github/Gallo_etal_2023_APWP_construction/data/vgp_database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BDDF86D-308A-7A49-86B2-81F00DA9075B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40B4C22D-442C-F44C-8DEA-1BE027E47E3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4260" yWindow="500" windowWidth="33600" windowHeight="19360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark2" sheetId="1" r:id="rId1"/>
@@ -554,9 +554,6 @@
     <t>Sediment Layer</t>
   </si>
   <si>
-    <t>Mudstone: Siltsone: Sandstone</t>
-  </si>
-  <si>
     <t>10.1130/B26104.1</t>
   </si>
   <si>
@@ -834,6 +831,9 @@
   </si>
   <si>
     <t>10.1130/B26104.93</t>
+  </si>
+  <si>
+    <t>Mudstone: Siltstone: Sandstone</t>
   </si>
 </sst>
 </file>
@@ -1230,8 +1230,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AQ1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y88" workbookViewId="0">
-      <selection activeCell="AP9" sqref="AP9:AP101"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
+      <selection activeCell="AB9" sqref="AB9:AB101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1899,7 +1899,7 @@
         <v>171</v>
       </c>
       <c r="AB9" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC9" s="9" t="s">
         <v>65</v>
@@ -1939,7 +1939,7 @@
         <v>67</v>
       </c>
       <c r="AP9" s="22" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="AQ9" s="6"/>
     </row>
@@ -2012,7 +2012,7 @@
         <v>171</v>
       </c>
       <c r="AB10" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC10" s="9" t="s">
         <v>65</v>
@@ -2050,7 +2050,7 @@
         <v>67</v>
       </c>
       <c r="AP10" s="22" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="AQ10" s="6"/>
     </row>
@@ -2123,7 +2123,7 @@
         <v>171</v>
       </c>
       <c r="AB11" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC11" s="9" t="s">
         <v>65</v>
@@ -2161,7 +2161,7 @@
         <v>67</v>
       </c>
       <c r="AP11" s="22" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="AQ11" s="6"/>
     </row>
@@ -2234,7 +2234,7 @@
         <v>171</v>
       </c>
       <c r="AB12" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC12" s="9" t="s">
         <v>65</v>
@@ -2272,7 +2272,7 @@
         <v>67</v>
       </c>
       <c r="AP12" s="22" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AQ12" s="6"/>
     </row>
@@ -2345,7 +2345,7 @@
         <v>171</v>
       </c>
       <c r="AB13" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC13" s="9" t="s">
         <v>65</v>
@@ -2383,7 +2383,7 @@
         <v>67</v>
       </c>
       <c r="AP13" s="22" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="AQ13" s="6"/>
     </row>
@@ -2456,7 +2456,7 @@
         <v>171</v>
       </c>
       <c r="AB14" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC14" s="9" t="s">
         <v>65</v>
@@ -2494,7 +2494,7 @@
         <v>67</v>
       </c>
       <c r="AP14" s="22" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AQ14" s="6"/>
     </row>
@@ -2567,7 +2567,7 @@
         <v>171</v>
       </c>
       <c r="AB15" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC15" s="9" t="s">
         <v>65</v>
@@ -2605,7 +2605,7 @@
         <v>67</v>
       </c>
       <c r="AP15" s="22" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AQ15" s="6"/>
     </row>
@@ -2678,7 +2678,7 @@
         <v>171</v>
       </c>
       <c r="AB16" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC16" s="9" t="s">
         <v>65</v>
@@ -2716,7 +2716,7 @@
         <v>67</v>
       </c>
       <c r="AP16" s="22" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="AQ16" s="6"/>
     </row>
@@ -2789,7 +2789,7 @@
         <v>171</v>
       </c>
       <c r="AB17" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC17" s="9" t="s">
         <v>65</v>
@@ -2831,7 +2831,7 @@
         <v>67</v>
       </c>
       <c r="AP17" s="22" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AQ17" s="6"/>
     </row>
@@ -2904,7 +2904,7 @@
         <v>171</v>
       </c>
       <c r="AB18" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC18" s="9" t="s">
         <v>65</v>
@@ -2942,7 +2942,7 @@
         <v>67</v>
       </c>
       <c r="AP18" s="22" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="AQ18" s="6"/>
     </row>
@@ -3015,7 +3015,7 @@
         <v>171</v>
       </c>
       <c r="AB19" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC19" s="9" t="s">
         <v>65</v>
@@ -3057,7 +3057,7 @@
         <v>67</v>
       </c>
       <c r="AP19" s="22" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AQ19" s="6"/>
     </row>
@@ -3130,7 +3130,7 @@
         <v>171</v>
       </c>
       <c r="AB20" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC20" s="9" t="s">
         <v>65</v>
@@ -3172,7 +3172,7 @@
         <v>67</v>
       </c>
       <c r="AP20" s="22" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AQ20" s="6"/>
     </row>
@@ -3245,7 +3245,7 @@
         <v>171</v>
       </c>
       <c r="AB21" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC21" s="9" t="s">
         <v>65</v>
@@ -3287,7 +3287,7 @@
         <v>67</v>
       </c>
       <c r="AP21" s="22" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AQ21" s="6"/>
     </row>
@@ -3360,7 +3360,7 @@
         <v>171</v>
       </c>
       <c r="AB22" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC22" s="9" t="s">
         <v>65</v>
@@ -3402,7 +3402,7 @@
         <v>67</v>
       </c>
       <c r="AP22" s="22" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AQ22" s="6"/>
     </row>
@@ -3475,7 +3475,7 @@
         <v>171</v>
       </c>
       <c r="AB23" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC23" s="9" t="s">
         <v>65</v>
@@ -3517,7 +3517,7 @@
         <v>67</v>
       </c>
       <c r="AP23" s="22" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AQ23" s="6"/>
     </row>
@@ -3590,7 +3590,7 @@
         <v>171</v>
       </c>
       <c r="AB24" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC24" s="9" t="s">
         <v>65</v>
@@ -3628,7 +3628,7 @@
         <v>67</v>
       </c>
       <c r="AP24" s="22" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AQ24" s="6"/>
     </row>
@@ -3701,7 +3701,7 @@
         <v>171</v>
       </c>
       <c r="AB25" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC25" s="9" t="s">
         <v>65</v>
@@ -3739,7 +3739,7 @@
         <v>67</v>
       </c>
       <c r="AP25" s="22" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AQ25" s="6"/>
     </row>
@@ -3812,7 +3812,7 @@
         <v>171</v>
       </c>
       <c r="AB26" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC26" s="9" t="s">
         <v>65</v>
@@ -3850,7 +3850,7 @@
         <v>67</v>
       </c>
       <c r="AP26" s="22" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AQ26" s="6"/>
     </row>
@@ -3923,7 +3923,7 @@
         <v>171</v>
       </c>
       <c r="AB27" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC27" s="9" t="s">
         <v>65</v>
@@ -3965,7 +3965,7 @@
         <v>67</v>
       </c>
       <c r="AP27" s="22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="AQ27" s="6"/>
     </row>
@@ -4038,7 +4038,7 @@
         <v>171</v>
       </c>
       <c r="AB28" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC28" s="9" t="s">
         <v>65</v>
@@ -4076,7 +4076,7 @@
         <v>67</v>
       </c>
       <c r="AP28" s="22" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="AQ28" s="6"/>
     </row>
@@ -4149,7 +4149,7 @@
         <v>171</v>
       </c>
       <c r="AB29" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC29" s="9" t="s">
         <v>65</v>
@@ -4187,7 +4187,7 @@
         <v>67</v>
       </c>
       <c r="AP29" s="22" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AQ29" s="6"/>
     </row>
@@ -4260,7 +4260,7 @@
         <v>171</v>
       </c>
       <c r="AB30" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC30" s="9" t="s">
         <v>65</v>
@@ -4298,7 +4298,7 @@
         <v>67</v>
       </c>
       <c r="AP30" s="22" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AQ30" s="6"/>
     </row>
@@ -4371,7 +4371,7 @@
         <v>171</v>
       </c>
       <c r="AB31" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC31" s="9" t="s">
         <v>65</v>
@@ -4409,7 +4409,7 @@
         <v>67</v>
       </c>
       <c r="AP31" s="22" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="AQ31" s="6"/>
     </row>
@@ -4482,7 +4482,7 @@
         <v>171</v>
       </c>
       <c r="AB32" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC32" s="9" t="s">
         <v>65</v>
@@ -4520,7 +4520,7 @@
         <v>92</v>
       </c>
       <c r="AP32" s="22" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AQ32" s="6"/>
     </row>
@@ -4593,7 +4593,7 @@
         <v>171</v>
       </c>
       <c r="AB33" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC33" s="9" t="s">
         <v>65</v>
@@ -4631,7 +4631,7 @@
         <v>92</v>
       </c>
       <c r="AP33" s="22" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="AQ33" s="6"/>
     </row>
@@ -4704,7 +4704,7 @@
         <v>171</v>
       </c>
       <c r="AB34" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC34" s="9" t="s">
         <v>65</v>
@@ -4742,7 +4742,7 @@
         <v>92</v>
       </c>
       <c r="AP34" s="22" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="AQ34" s="6"/>
     </row>
@@ -4815,7 +4815,7 @@
         <v>171</v>
       </c>
       <c r="AB35" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC35" s="9" t="s">
         <v>65</v>
@@ -4853,7 +4853,7 @@
         <v>92</v>
       </c>
       <c r="AP35" s="22" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AQ35" s="6"/>
     </row>
@@ -4926,7 +4926,7 @@
         <v>171</v>
       </c>
       <c r="AB36" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC36" s="9" t="s">
         <v>65</v>
@@ -4964,7 +4964,7 @@
         <v>92</v>
       </c>
       <c r="AP36" s="22" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AQ36" s="6"/>
     </row>
@@ -5037,7 +5037,7 @@
         <v>171</v>
       </c>
       <c r="AB37" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC37" s="9" t="s">
         <v>65</v>
@@ -5075,7 +5075,7 @@
         <v>92</v>
       </c>
       <c r="AP37" s="22" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AQ37" s="6"/>
     </row>
@@ -5148,7 +5148,7 @@
         <v>171</v>
       </c>
       <c r="AB38" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC38" s="9" t="s">
         <v>65</v>
@@ -5186,7 +5186,7 @@
         <v>92</v>
       </c>
       <c r="AP38" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AQ38" s="6"/>
     </row>
@@ -5259,7 +5259,7 @@
         <v>171</v>
       </c>
       <c r="AB39" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC39" s="9" t="s">
         <v>65</v>
@@ -5297,7 +5297,7 @@
         <v>92</v>
       </c>
       <c r="AP39" s="22" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AQ39" s="6"/>
     </row>
@@ -5370,7 +5370,7 @@
         <v>171</v>
       </c>
       <c r="AB40" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC40" s="9" t="s">
         <v>65</v>
@@ -5408,7 +5408,7 @@
         <v>92</v>
       </c>
       <c r="AP40" s="22" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="AQ40" s="6"/>
     </row>
@@ -5481,7 +5481,7 @@
         <v>171</v>
       </c>
       <c r="AB41" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC41" s="9" t="s">
         <v>65</v>
@@ -5519,7 +5519,7 @@
         <v>92</v>
       </c>
       <c r="AP41" s="22" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="AQ41" s="6"/>
     </row>
@@ -5592,7 +5592,7 @@
         <v>171</v>
       </c>
       <c r="AB42" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC42" s="9" t="s">
         <v>65</v>
@@ -5630,7 +5630,7 @@
         <v>92</v>
       </c>
       <c r="AP42" s="22" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="AQ42" s="6"/>
     </row>
@@ -5703,7 +5703,7 @@
         <v>171</v>
       </c>
       <c r="AB43" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC43" s="9" t="s">
         <v>65</v>
@@ -5741,7 +5741,7 @@
         <v>92</v>
       </c>
       <c r="AP43" s="22" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AQ43" s="6"/>
     </row>
@@ -5814,7 +5814,7 @@
         <v>171</v>
       </c>
       <c r="AB44" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC44" s="9" t="s">
         <v>65</v>
@@ -5852,7 +5852,7 @@
         <v>92</v>
       </c>
       <c r="AP44" s="22" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AQ44" s="6"/>
     </row>
@@ -5925,7 +5925,7 @@
         <v>171</v>
       </c>
       <c r="AB45" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC45" s="9" t="s">
         <v>65</v>
@@ -5963,7 +5963,7 @@
         <v>92</v>
       </c>
       <c r="AP45" s="22" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AQ45" s="6"/>
     </row>
@@ -6036,7 +6036,7 @@
         <v>171</v>
       </c>
       <c r="AB46" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC46" s="9" t="s">
         <v>65</v>
@@ -6078,7 +6078,7 @@
         <v>92</v>
       </c>
       <c r="AP46" s="22" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="AQ46" s="6"/>
     </row>
@@ -6151,7 +6151,7 @@
         <v>171</v>
       </c>
       <c r="AB47" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC47" s="9" t="s">
         <v>65</v>
@@ -6193,7 +6193,7 @@
         <v>92</v>
       </c>
       <c r="AP47" s="22" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AQ47" s="6"/>
     </row>
@@ -6266,7 +6266,7 @@
         <v>171</v>
       </c>
       <c r="AB48" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC48" s="9" t="s">
         <v>65</v>
@@ -6304,7 +6304,7 @@
         <v>109</v>
       </c>
       <c r="AP48" s="22" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="AQ48" s="6"/>
     </row>
@@ -6377,7 +6377,7 @@
         <v>171</v>
       </c>
       <c r="AB49" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC49" s="9" t="s">
         <v>65</v>
@@ -6415,7 +6415,7 @@
         <v>109</v>
       </c>
       <c r="AP49" s="22" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="AQ49" s="6"/>
     </row>
@@ -6488,7 +6488,7 @@
         <v>171</v>
       </c>
       <c r="AB50" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC50" s="9" t="s">
         <v>65</v>
@@ -6526,7 +6526,7 @@
         <v>109</v>
       </c>
       <c r="AP50" s="22" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="AQ50" s="6"/>
     </row>
@@ -6599,7 +6599,7 @@
         <v>171</v>
       </c>
       <c r="AB51" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC51" s="9" t="s">
         <v>65</v>
@@ -6637,7 +6637,7 @@
         <v>109</v>
       </c>
       <c r="AP51" s="22" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="AQ51" s="6"/>
     </row>
@@ -6710,7 +6710,7 @@
         <v>171</v>
       </c>
       <c r="AB52" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC52" s="9" t="s">
         <v>65</v>
@@ -6752,7 +6752,7 @@
         <v>109</v>
       </c>
       <c r="AP52" s="22" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AQ52" s="6"/>
     </row>
@@ -6825,7 +6825,7 @@
         <v>171</v>
       </c>
       <c r="AB53" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC53" s="9" t="s">
         <v>65</v>
@@ -6867,7 +6867,7 @@
         <v>109</v>
       </c>
       <c r="AP53" s="22" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="AQ53" s="6"/>
     </row>
@@ -6940,7 +6940,7 @@
         <v>171</v>
       </c>
       <c r="AB54" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC54" s="9" t="s">
         <v>65</v>
@@ -6982,7 +6982,7 @@
         <v>109</v>
       </c>
       <c r="AP54" s="22" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AQ54" s="6"/>
     </row>
@@ -7055,7 +7055,7 @@
         <v>171</v>
       </c>
       <c r="AB55" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC55" s="9" t="s">
         <v>65</v>
@@ -7093,7 +7093,7 @@
         <v>109</v>
       </c>
       <c r="AP55" s="22" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AQ55" s="6"/>
     </row>
@@ -7166,7 +7166,7 @@
         <v>171</v>
       </c>
       <c r="AB56" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC56" s="9" t="s">
         <v>65</v>
@@ -7204,7 +7204,7 @@
         <v>109</v>
       </c>
       <c r="AP56" s="22" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="AQ56" s="6"/>
     </row>
@@ -7277,7 +7277,7 @@
         <v>171</v>
       </c>
       <c r="AB57" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC57" s="9" t="s">
         <v>65</v>
@@ -7315,7 +7315,7 @@
         <v>109</v>
       </c>
       <c r="AP57" s="22" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AQ57" s="6"/>
     </row>
@@ -7388,7 +7388,7 @@
         <v>171</v>
       </c>
       <c r="AB58" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC58" s="9" t="s">
         <v>65</v>
@@ -7430,7 +7430,7 @@
         <v>109</v>
       </c>
       <c r="AP58" s="22" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="AQ58" s="6"/>
     </row>
@@ -7503,7 +7503,7 @@
         <v>171</v>
       </c>
       <c r="AB59" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC59" s="9" t="s">
         <v>65</v>
@@ -7545,7 +7545,7 @@
         <v>109</v>
       </c>
       <c r="AP59" s="22" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AQ59" s="6"/>
     </row>
@@ -7618,7 +7618,7 @@
         <v>171</v>
       </c>
       <c r="AB60" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC60" s="9" t="s">
         <v>65</v>
@@ -7656,7 +7656,7 @@
         <v>109</v>
       </c>
       <c r="AP60" s="22" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="AQ60" s="6"/>
     </row>
@@ -7729,7 +7729,7 @@
         <v>171</v>
       </c>
       <c r="AB61" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC61" s="9" t="s">
         <v>65</v>
@@ -7767,7 +7767,7 @@
         <v>109</v>
       </c>
       <c r="AP61" s="22" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="AQ61" s="6"/>
     </row>
@@ -7840,7 +7840,7 @@
         <v>171</v>
       </c>
       <c r="AB62" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC62" s="9" t="s">
         <v>65</v>
@@ -7878,7 +7878,7 @@
         <v>109</v>
       </c>
       <c r="AP62" s="22" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="AQ62" s="6"/>
     </row>
@@ -7951,7 +7951,7 @@
         <v>171</v>
       </c>
       <c r="AB63" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC63" s="9" t="s">
         <v>65</v>
@@ -7989,7 +7989,7 @@
         <v>109</v>
       </c>
       <c r="AP63" s="22" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="AQ63" s="6"/>
     </row>
@@ -8062,7 +8062,7 @@
         <v>171</v>
       </c>
       <c r="AB64" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC64" s="9" t="s">
         <v>65</v>
@@ -8100,7 +8100,7 @@
         <v>109</v>
       </c>
       <c r="AP64" s="22" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AQ64" s="6"/>
     </row>
@@ -8173,7 +8173,7 @@
         <v>171</v>
       </c>
       <c r="AB65" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC65" s="9" t="s">
         <v>65</v>
@@ -8211,7 +8211,7 @@
         <v>109</v>
       </c>
       <c r="AP65" s="22" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="AQ65" s="6"/>
     </row>
@@ -8284,7 +8284,7 @@
         <v>171</v>
       </c>
       <c r="AB66" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC66" s="9" t="s">
         <v>65</v>
@@ -8326,7 +8326,7 @@
         <v>109</v>
       </c>
       <c r="AP66" s="22" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="AQ66" s="6"/>
     </row>
@@ -8399,7 +8399,7 @@
         <v>171</v>
       </c>
       <c r="AB67" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC67" s="9" t="s">
         <v>65</v>
@@ -8437,7 +8437,7 @@
         <v>109</v>
       </c>
       <c r="AP67" s="22" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="AQ67" s="6"/>
     </row>
@@ -8510,7 +8510,7 @@
         <v>171</v>
       </c>
       <c r="AB68" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC68" s="9" t="s">
         <v>65</v>
@@ -8552,7 +8552,7 @@
         <v>109</v>
       </c>
       <c r="AP68" s="22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="AQ68" s="6"/>
     </row>
@@ -8625,7 +8625,7 @@
         <v>171</v>
       </c>
       <c r="AB69" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC69" s="9" t="s">
         <v>65</v>
@@ -8663,7 +8663,7 @@
         <v>109</v>
       </c>
       <c r="AP69" s="22" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="AQ69" s="6"/>
     </row>
@@ -8736,7 +8736,7 @@
         <v>171</v>
       </c>
       <c r="AB70" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC70" s="9" t="s">
         <v>65</v>
@@ -8778,7 +8778,7 @@
         <v>109</v>
       </c>
       <c r="AP70" s="22" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AQ70" s="6"/>
     </row>
@@ -8851,7 +8851,7 @@
         <v>171</v>
       </c>
       <c r="AB71" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC71" s="9" t="s">
         <v>65</v>
@@ -8893,7 +8893,7 @@
         <v>109</v>
       </c>
       <c r="AP71" s="22" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="AQ71" s="6"/>
     </row>
@@ -8966,7 +8966,7 @@
         <v>171</v>
       </c>
       <c r="AB72" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC72" s="9" t="s">
         <v>65</v>
@@ -9008,7 +9008,7 @@
         <v>109</v>
       </c>
       <c r="AP72" s="22" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="AQ72" s="6"/>
     </row>
@@ -9081,7 +9081,7 @@
         <v>171</v>
       </c>
       <c r="AB73" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC73" s="9" t="s">
         <v>65</v>
@@ -9119,7 +9119,7 @@
         <v>136</v>
       </c>
       <c r="AP73" s="22" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AQ73" s="6"/>
     </row>
@@ -9192,7 +9192,7 @@
         <v>171</v>
       </c>
       <c r="AB74" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC74" s="9" t="s">
         <v>65</v>
@@ -9234,7 +9234,7 @@
         <v>136</v>
       </c>
       <c r="AP74" s="22" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="AQ74" s="6"/>
     </row>
@@ -9307,7 +9307,7 @@
         <v>171</v>
       </c>
       <c r="AB75" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC75" s="9" t="s">
         <v>65</v>
@@ -9349,7 +9349,7 @@
         <v>136</v>
       </c>
       <c r="AP75" s="22" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AQ75" s="6"/>
     </row>
@@ -9422,7 +9422,7 @@
         <v>171</v>
       </c>
       <c r="AB76" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC76" s="9" t="s">
         <v>65</v>
@@ -9464,7 +9464,7 @@
         <v>136</v>
       </c>
       <c r="AP76" s="22" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="AQ76" s="6"/>
     </row>
@@ -9537,7 +9537,7 @@
         <v>171</v>
       </c>
       <c r="AB77" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC77" s="9" t="s">
         <v>65</v>
@@ -9575,7 +9575,7 @@
         <v>136</v>
       </c>
       <c r="AP77" s="22" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="AQ77" s="6"/>
     </row>
@@ -9648,7 +9648,7 @@
         <v>171</v>
       </c>
       <c r="AB78" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC78" s="9" t="s">
         <v>65</v>
@@ -9690,7 +9690,7 @@
         <v>136</v>
       </c>
       <c r="AP78" s="22" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="AQ78" s="6"/>
     </row>
@@ -9763,7 +9763,7 @@
         <v>171</v>
       </c>
       <c r="AB79" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC79" s="9" t="s">
         <v>65</v>
@@ -9801,7 +9801,7 @@
         <v>136</v>
       </c>
       <c r="AP79" s="22" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="AQ79" s="6"/>
     </row>
@@ -9874,7 +9874,7 @@
         <v>171</v>
       </c>
       <c r="AB80" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC80" s="9" t="s">
         <v>65</v>
@@ -9912,7 +9912,7 @@
         <v>144</v>
       </c>
       <c r="AP80" s="22" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="AQ80" s="6"/>
     </row>
@@ -9985,7 +9985,7 @@
         <v>171</v>
       </c>
       <c r="AB81" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC81" s="9" t="s">
         <v>65</v>
@@ -10027,7 +10027,7 @@
         <v>144</v>
       </c>
       <c r="AP81" s="22" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="AQ81" s="6"/>
     </row>
@@ -10100,7 +10100,7 @@
         <v>171</v>
       </c>
       <c r="AB82" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC82" s="9" t="s">
         <v>65</v>
@@ -10138,7 +10138,7 @@
         <v>144</v>
       </c>
       <c r="AP82" s="22" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="AQ82" s="6"/>
     </row>
@@ -10211,7 +10211,7 @@
         <v>171</v>
       </c>
       <c r="AB83" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC83" s="9" t="s">
         <v>65</v>
@@ -10253,7 +10253,7 @@
         <v>144</v>
       </c>
       <c r="AP83" s="22" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="AQ83" s="6"/>
     </row>
@@ -10326,7 +10326,7 @@
         <v>171</v>
       </c>
       <c r="AB84" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC84" s="9" t="s">
         <v>65</v>
@@ -10368,7 +10368,7 @@
         <v>144</v>
       </c>
       <c r="AP84" s="22" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="AQ84" s="6"/>
     </row>
@@ -10441,7 +10441,7 @@
         <v>171</v>
       </c>
       <c r="AB85" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC85" s="9" t="s">
         <v>65</v>
@@ -10483,7 +10483,7 @@
         <v>144</v>
       </c>
       <c r="AP85" s="22" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="AQ85" s="6"/>
     </row>
@@ -10556,7 +10556,7 @@
         <v>171</v>
       </c>
       <c r="AB86" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC86" s="9" t="s">
         <v>65</v>
@@ -10598,7 +10598,7 @@
         <v>144</v>
       </c>
       <c r="AP86" s="22" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="AQ86" s="6"/>
     </row>
@@ -10671,7 +10671,7 @@
         <v>171</v>
       </c>
       <c r="AB87" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC87" s="9" t="s">
         <v>65</v>
@@ -10709,7 +10709,7 @@
         <v>144</v>
       </c>
       <c r="AP87" s="22" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="AQ87" s="6"/>
     </row>
@@ -10782,7 +10782,7 @@
         <v>171</v>
       </c>
       <c r="AB88" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC88" s="9" t="s">
         <v>65</v>
@@ -10820,7 +10820,7 @@
         <v>144</v>
       </c>
       <c r="AP88" s="22" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="AQ88" s="6"/>
     </row>
@@ -10893,7 +10893,7 @@
         <v>171</v>
       </c>
       <c r="AB89" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC89" s="9" t="s">
         <v>65</v>
@@ -10935,7 +10935,7 @@
         <v>144</v>
       </c>
       <c r="AP89" s="22" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="AQ89" s="6"/>
     </row>
@@ -11008,7 +11008,7 @@
         <v>171</v>
       </c>
       <c r="AB90" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC90" s="9" t="s">
         <v>65</v>
@@ -11050,7 +11050,7 @@
         <v>144</v>
       </c>
       <c r="AP90" s="22" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="AQ90" s="6"/>
     </row>
@@ -11123,7 +11123,7 @@
         <v>171</v>
       </c>
       <c r="AB91" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC91" s="9" t="s">
         <v>65</v>
@@ -11165,7 +11165,7 @@
         <v>144</v>
       </c>
       <c r="AP91" s="22" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="AQ91" s="6"/>
     </row>
@@ -11238,7 +11238,7 @@
         <v>171</v>
       </c>
       <c r="AB92" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC92" s="9" t="s">
         <v>65</v>
@@ -11280,7 +11280,7 @@
         <v>144</v>
       </c>
       <c r="AP92" s="22" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="AQ92" s="6"/>
     </row>
@@ -11353,7 +11353,7 @@
         <v>171</v>
       </c>
       <c r="AB93" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC93" s="9" t="s">
         <v>65</v>
@@ -11391,7 +11391,7 @@
         <v>144</v>
       </c>
       <c r="AP93" s="22" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="AQ93" s="6"/>
     </row>
@@ -11464,7 +11464,7 @@
         <v>171</v>
       </c>
       <c r="AB94" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC94" s="9" t="s">
         <v>65</v>
@@ -11502,7 +11502,7 @@
         <v>144</v>
       </c>
       <c r="AP94" s="22" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="AQ94" s="6"/>
     </row>
@@ -11575,7 +11575,7 @@
         <v>171</v>
       </c>
       <c r="AB95" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC95" s="9" t="s">
         <v>65</v>
@@ -11617,7 +11617,7 @@
         <v>144</v>
       </c>
       <c r="AP95" s="22" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="AQ95" s="6"/>
     </row>
@@ -11690,7 +11690,7 @@
         <v>171</v>
       </c>
       <c r="AB96" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC96" s="9" t="s">
         <v>65</v>
@@ -11728,7 +11728,7 @@
         <v>144</v>
       </c>
       <c r="AP96" s="22" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="AQ96" s="6"/>
     </row>
@@ -11801,7 +11801,7 @@
         <v>171</v>
       </c>
       <c r="AB97" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC97" s="9" t="s">
         <v>65</v>
@@ -11839,7 +11839,7 @@
         <v>144</v>
       </c>
       <c r="AP97" s="22" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="AQ97" s="6"/>
     </row>
@@ -11912,7 +11912,7 @@
         <v>171</v>
       </c>
       <c r="AB98" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC98" s="9" t="s">
         <v>65</v>
@@ -11950,7 +11950,7 @@
         <v>144</v>
       </c>
       <c r="AP98" s="22" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="AQ98" s="6"/>
     </row>
@@ -12023,7 +12023,7 @@
         <v>171</v>
       </c>
       <c r="AB99" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC99" s="9" t="s">
         <v>65</v>
@@ -12061,7 +12061,7 @@
         <v>144</v>
       </c>
       <c r="AP99" s="22" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="AQ99" s="6"/>
     </row>
@@ -12134,7 +12134,7 @@
         <v>171</v>
       </c>
       <c r="AB100" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC100" s="9" t="s">
         <v>65</v>
@@ -12172,7 +12172,7 @@
         <v>144</v>
       </c>
       <c r="AP100" s="22" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="AQ100" s="6"/>
     </row>
@@ -12245,7 +12245,7 @@
         <v>171</v>
       </c>
       <c r="AB101" s="9" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="AC101" s="9" t="s">
         <v>65</v>
@@ -12283,7 +12283,7 @@
         <v>144</v>
       </c>
       <c r="AP101" s="22" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="AQ101" s="6"/>
     </row>

</xml_diff>